<commit_message>
updated pinout name BUZZER-> PIEZO
</commit_message>
<xml_diff>
--- a/kit_pinout.xlsx
+++ b/kit_pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejponcak/repos/dp/pico-kit-pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8972A919-4494-2541-986A-B507BD221A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B921A8A-68E8-554E-BC06-2954883E1F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4840" yWindow="-16000" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -175,39 +175,12 @@
     <t>ENC_BUTTON</t>
   </si>
   <si>
-    <t>SPI RX</t>
-  </si>
-  <si>
-    <t>SPI CS</t>
-  </si>
-  <si>
     <t>LED1/SPI SCK</t>
   </si>
   <si>
-    <t>LED2/SPI TX</t>
-  </si>
-  <si>
     <t>POTENTIOMETER</t>
   </si>
   <si>
-    <t>ENC_SW</t>
-  </si>
-  <si>
-    <t>SPI_LOAD</t>
-  </si>
-  <si>
-    <t>LED3/L/I2S_LRCK</t>
-  </si>
-  <si>
-    <t>LED4/R/I2S_BCK</t>
-  </si>
-  <si>
-    <t>BUZZER/I2S_DIN</t>
-  </si>
-  <si>
-    <t>VGA_B0</t>
-  </si>
-  <si>
     <t>VGA_B1/DVI_D0+</t>
   </si>
   <si>
@@ -233,6 +206,33 @@
   </si>
   <si>
     <t>VGA_VSYNC</t>
+  </si>
+  <si>
+    <t>SPI RX (MISO)</t>
+  </si>
+  <si>
+    <t>SPI SD CS</t>
+  </si>
+  <si>
+    <t>LED2/SPI TX (MOSI)</t>
+  </si>
+  <si>
+    <t>LED3/PWM L/I2S_LRCK</t>
+  </si>
+  <si>
+    <t>LED4/PWM R/I2S_BCK</t>
+  </si>
+  <si>
+    <t>VGA_B0/ENC_SW</t>
+  </si>
+  <si>
+    <t>SPI EXPANDER CS</t>
+  </si>
+  <si>
+    <t>DAC_BUTTONS</t>
+  </si>
+  <si>
+    <t>PIEZO/I2S_DIN</t>
   </si>
 </sst>
 </file>
@@ -964,13 +964,13 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
@@ -1057,7 +1057,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -1086,7 +1086,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
@@ -1105,7 +1105,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -1120,12 +1120,12 @@
         <v>13</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -1140,12 +1140,12 @@
         <v>15</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>16</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
@@ -1234,12 +1234,12 @@
         <v>23</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>24</v>
@@ -1254,12 +1254,12 @@
         <v>25</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>26</v>
@@ -1274,7 +1274,7 @@
         <v>27</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -1293,7 +1293,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>28</v>
@@ -1308,12 +1308,12 @@
         <v>29</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>30</v>
@@ -1328,7 +1328,7 @@
         <v>31</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>